<commit_message>
Notes on lab procedure from class on February 27, 2020
</commit_message>
<xml_diff>
--- a/Reference/Template_Table_SpatialDescriptiveStatistics.xlsx
+++ b/Reference/Template_Table_SpatialDescriptiveStatistics.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="DirectionalDistribution" sheetId="1" r:id="rId1"/>
+    <sheet name="SpatialAutocorrelation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Variable</t>
   </si>
@@ -91,7 +92,49 @@
     <t>Table #. Spatial Descriptive Statistics for the St. Louis Metropolitan Statistical Area</t>
   </si>
   <si>
-    <t>Source: U.S. Census ACS 2014-2018. Table created by Author.</t>
+    <t>Variable 1</t>
+  </si>
+  <si>
+    <t>Variable 2</t>
+  </si>
+  <si>
+    <t>Variable 3</t>
+  </si>
+  <si>
+    <t>Significance</t>
+  </si>
+  <si>
+    <t>Global Moran's I</t>
+  </si>
+  <si>
+    <t>***</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>*** p &lt; 0.001, ** p &lt; 0.01, * p &lt; 0.05</t>
+  </si>
+  <si>
+    <t>Queen method used for weight matrix.</t>
+  </si>
+  <si>
+    <t>Source: U.S. Census ACS 2014-2018 5-year estimate. Table created by Author.</t>
+  </si>
+  <si>
+    <t>Table #. Spatial Autocorrelation of Regression Model Variables</t>
+  </si>
+  <si>
+    <t>z-value</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t>Source: U.S. Census ACS 2014-2018 5-year estimates. Table created by Author.</t>
   </si>
 </sst>
 </file>
@@ -156,40 +199,55 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -508,7 +566,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,104 +577,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="A10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -628,4 +686,112 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+    </row>
+    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:E8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Homework01 spatial descriptive statistics tables
</commit_message>
<xml_diff>
--- a/Reference/Template_Table_SpatialDescriptiveStatistics.xlsx
+++ b/Reference/Template_Table_SpatialDescriptiveStatistics.xlsx
@@ -27,16 +27,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
-    <t>Variable</t>
-  </si>
-  <si>
     <t>Mean Center - X Coordinate</t>
   </si>
   <si>
     <t>Mean Center - Y Coordinate</t>
-  </si>
-  <si>
-    <t>Name</t>
   </si>
   <si>
     <t>White</t>
@@ -135,6 +129,12 @@
   </si>
   <si>
     <t>Source: U.S. Census ACS 2014-2018 5-year estimates. Table created by Author.</t>
+  </si>
+  <si>
+    <t>Spatical Statistic</t>
+  </si>
+  <si>
+    <t>Components</t>
   </si>
 </sst>
 </file>
@@ -199,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -223,9 +223,18 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -234,20 +243,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -577,46 +580,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="A1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>1</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -630,51 +633,51 @@
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>12</v>
+      <c r="A6" s="16" t="s">
+        <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -702,88 +705,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="A1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>14</v>
+      <c r="A3" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
-      <c r="E3" s="14" t="s">
-        <v>19</v>
+      <c r="E3" s="10" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>15</v>
+      <c r="A4" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="14" t="s">
-        <v>20</v>
+      <c r="E4" s="10" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>16</v>
+      <c r="A5" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>